<commit_message>
Commit on 10 Mar 2025
</commit_message>
<xml_diff>
--- a/src/main/java/Unifyed/Unifyed_Engage/Resources/dataDriven.xlsx
+++ b/src/main/java/Unifyed/Unifyed_Engage/Resources/dataDriven.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philip_parker\eclipse-workspace\Unifyed_Engage\src\main\java\Unifyed\Unifyed_Engage\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Unifyed_Engage\src\main\java\Unifyed\Unifyed_Engage\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E6EE1A-67A2-4578-A013-94DE325EED0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E99772C-8B23-4FC6-8083-78D2B96B15CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E1630F13-00CF-48B0-9ABA-1263F119782C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -48,12 +48,6 @@
   </si>
   <si>
     <t>Admin@2008</t>
-  </si>
-  <si>
-    <t>pankaj_kalra@unifyedqa.edu</t>
-  </si>
-  <si>
-    <t>Admin@2008s</t>
   </si>
 </sst>
 </file>
@@ -120,9 +114,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -160,7 +154,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -266,7 +260,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,7 +402,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -416,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5363A28F-909E-40D5-89E0-BCA7386866FC}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,26 +432,16 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{0A61BF2B-1378-4726-BEF2-1718A548D1FA}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{106F2EBD-E7C1-4120-90BA-EAF62D6F401F}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{7CC5AF9B-38CF-441A-99E0-439C6B0AAE18}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{CFDDFA83-D39F-45FF-AE77-6EBF18809BAB}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0A61BF2B-1378-4726-BEF2-1718A548D1FA}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{106F2EBD-E7C1-4120-90BA-EAF62D6F401F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>